<commit_message>
Added Experiment feature + bug fixes
</commit_message>
<xml_diff>
--- a/Frontend/src/App/data/countries.xlsx
+++ b/Frontend/src/App/data/countries.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mendy\Desktop\Projects\CareerBoost\CareerBoost\src\components\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mendy\Desktop\Projects\CareerBoost\CareerBoost\Frontend\src\App\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967C3F05-8819-443F-99E9-0D760302D275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26E6FC1-4F8D-49DC-9F4A-9DD37A74684B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Azerbaijan</t>
   </si>
   <si>
-    <t>Bahamas</t>
-  </si>
-  <si>
     <t>Bahrain</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>Belgium</t>
   </si>
   <si>
-    <t>Belize</t>
-  </si>
-  <si>
     <t>Benin</t>
   </si>
   <si>
@@ -129,9 +123,6 @@
     <t>Central African Republic</t>
   </si>
   <si>
-    <t>Chad</t>
-  </si>
-  <si>
     <t>Chile</t>
   </si>
   <si>
@@ -168,12 +159,6 @@
     <t>Denmark</t>
   </si>
   <si>
-    <t>Djibouti</t>
-  </si>
-  <si>
-    <t>Dominica</t>
-  </si>
-  <si>
     <t>Dominican Republic</t>
   </si>
   <si>
@@ -186,9 +171,6 @@
     <t>El Salvador</t>
   </si>
   <si>
-    <t>Equatorial Guinea</t>
-  </si>
-  <si>
     <t>Estonia</t>
   </si>
   <si>
@@ -216,21 +198,12 @@
     <t>Ghana</t>
   </si>
   <si>
-    <t>Grand Total</t>
-  </si>
-  <si>
     <t>Greece</t>
   </si>
   <si>
     <t>Guatemala</t>
   </si>
   <si>
-    <t>Guinea</t>
-  </si>
-  <si>
-    <t>Guinea-Bissau</t>
-  </si>
-  <si>
     <t>Guyana</t>
   </si>
   <si>
@@ -309,9 +282,6 @@
     <t>Lesotho</t>
   </si>
   <si>
-    <t>Liberia</t>
-  </si>
-  <si>
     <t>Libyan Arab Jamahiriya</t>
   </si>
   <si>
@@ -351,12 +321,6 @@
     <t>Mexico</t>
   </si>
   <si>
-    <t>Micronesia, Federated States of...</t>
-  </si>
-  <si>
-    <t>Monaco</t>
-  </si>
-  <si>
     <t>Mongolia</t>
   </si>
   <si>
@@ -372,15 +336,9 @@
     <t>Myanmar</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Namibia</t>
   </si>
   <si>
-    <t>Nauru</t>
-  </si>
-  <si>
     <t>Nepal</t>
   </si>
   <si>
@@ -393,18 +351,12 @@
     <t>Nicaragua</t>
   </si>
   <si>
-    <t>Niger</t>
-  </si>
-  <si>
     <t>Nigeria</t>
   </si>
   <si>
     <t>Nomadic</t>
   </si>
   <si>
-    <t>North Korea</t>
-  </si>
-  <si>
     <t>Norway</t>
   </si>
   <si>
@@ -420,9 +372,6 @@
     <t>Panama</t>
   </si>
   <si>
-    <t>Papua New Guinea</t>
-  </si>
-  <si>
     <t>Paraguay</t>
   </si>
   <si>
@@ -459,15 +408,9 @@
     <t>Rwanda</t>
   </si>
   <si>
-    <t>Saint Kitts and Nevis</t>
-  </si>
-  <si>
     <t>Samoa</t>
   </si>
   <si>
-    <t>San Marino</t>
-  </si>
-  <si>
     <t>Saudi Arabia</t>
   </si>
   <si>
@@ -489,9 +432,6 @@
     <t>Slovenia</t>
   </si>
   <si>
-    <t>Solomon Islands</t>
-  </si>
-  <si>
     <t>Somalia</t>
   </si>
   <si>
@@ -511,9 +451,6 @@
   </si>
   <si>
     <t>Suriname</t>
-  </si>
-  <si>
-    <t>Swaziland</t>
   </si>
   <si>
     <t>Sweden</t>
@@ -903,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A187"/>
+  <dimension ref="A1:A166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A167" sqref="A167:A187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1744,111 +1681,6 @@
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A167" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A168" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A169" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A170" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A171" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A172" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A173" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A174" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A175" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A176" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A177" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A178" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A179" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A180" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A181" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A182" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A183" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A184" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A185" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A186" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A187" t="s">
-        <v>186</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>